<commit_message>
añadido mejoras de sistema de mensajes y alertas
</commit_message>
<xml_diff>
--- a/ventas_v2.xlsx
+++ b/ventas_v2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
@@ -404,7 +404,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>H29468279</v>
+        <v>H29485893</v>
       </c>
       <c r="B1" t="str">
         <v>terminado</v>
@@ -412,7 +412,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>H29474657</v>
+        <v>H29498961</v>
       </c>
       <c r="B2" t="str">
         <v>terminado</v>
@@ -420,15 +420,24 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>H29479748</v>
+        <v>H29531290</v>
       </c>
       <c r="B3" t="str">
-        <v>terminado</v>
+        <v>corregir</v>
+      </c>
+      <c r="C3" t="str">
+        <v/>
+      </c>
+      <c r="D3" t="str">
+        <v/>
+      </c>
+      <c r="E3" t="str">
+        <v/>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>H29480829</v>
+        <v>H29552494</v>
       </c>
       <c r="B4" t="str">
         <v>terminado</v>
@@ -436,7 +445,7 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>H29483088</v>
+        <v>H29552791</v>
       </c>
       <c r="B5" t="str">
         <v>terminado</v>
@@ -444,7 +453,7 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>H29483252</v>
+        <v>H29552908</v>
       </c>
       <c r="B6" t="str">
         <v>terminado</v>
@@ -452,7 +461,7 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>H29485299</v>
+        <v>H29568474</v>
       </c>
       <c r="B7" t="str">
         <v>terminado</v>
@@ -460,7 +469,7 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>H29485893</v>
+        <v>H29617552</v>
       </c>
       <c r="B8" t="str">
         <v>terminado</v>
@@ -468,7 +477,7 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>H29487170</v>
+        <v>H29634433</v>
       </c>
       <c r="B9" t="str">
         <v>terminado</v>
@@ -476,7 +485,7 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>H29496718</v>
+        <v>H29674926</v>
       </c>
       <c r="B10" t="str">
         <v>terminado</v>
@@ -484,10 +493,10 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>H28644029</v>
+        <v/>
       </c>
       <c r="B11" t="str">
-        <v>corregir</v>
+        <v/>
       </c>
       <c r="C11" t="str">
         <v/>
@@ -501,10 +510,10 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>H25520222</v>
+        <v/>
       </c>
       <c r="B12" t="str">
-        <v>corregir</v>
+        <v/>
       </c>
       <c r="C12" t="str">
         <v/>
@@ -518,10 +527,10 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>H25483231</v>
+        <v/>
       </c>
       <c r="B13" t="str">
-        <v>corregir</v>
+        <v/>
       </c>
       <c r="C13" t="str">
         <v/>

</xml_diff>

<commit_message>
añadido verificacion de workcenter
</commit_message>
<xml_diff>
--- a/ventas_v2.xlsx
+++ b/ventas_v2.xlsx
@@ -404,91 +404,163 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>H29485893</v>
+        <v>H59388249</v>
       </c>
       <c r="B1" t="str">
-        <v>terminado</v>
+        <v>workcenter</v>
+      </c>
+      <c r="C1" t="str">
+        <v/>
+      </c>
+      <c r="D1" t="str">
+        <v/>
+      </c>
+      <c r="E1" t="str">
+        <v/>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>H29498961</v>
+        <v>H59384552</v>
       </c>
       <c r="B2" t="str">
-        <v>terminado</v>
+        <v>workcenter</v>
+      </c>
+      <c r="C2" t="str">
+        <v/>
+      </c>
+      <c r="D2" t="str">
+        <v/>
+      </c>
+      <c r="E2" t="str">
+        <v/>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>H29531290</v>
+        <v>H59392720</v>
       </c>
       <c r="B3" t="str">
-        <v>corregir</v>
-      </c>
-      <c r="C3" t="str">
-        <v/>
-      </c>
-      <c r="D3" t="str">
-        <v/>
-      </c>
-      <c r="E3" t="str">
-        <v/>
+        <v>correcta_por_defecto</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>H29552494</v>
+        <v/>
       </c>
       <c r="B4" t="str">
-        <v>terminado</v>
+        <v/>
+      </c>
+      <c r="C4" t="str">
+        <v/>
+      </c>
+      <c r="D4" t="str">
+        <v/>
+      </c>
+      <c r="E4" t="str">
+        <v/>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>H29552791</v>
+        <v/>
       </c>
       <c r="B5" t="str">
-        <v>terminado</v>
+        <v/>
+      </c>
+      <c r="C5" t="str">
+        <v/>
+      </c>
+      <c r="D5" t="str">
+        <v/>
+      </c>
+      <c r="E5" t="str">
+        <v/>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>H29552908</v>
+        <v/>
       </c>
       <c r="B6" t="str">
-        <v>terminado</v>
+        <v/>
+      </c>
+      <c r="C6" t="str">
+        <v/>
+      </c>
+      <c r="D6" t="str">
+        <v/>
+      </c>
+      <c r="E6" t="str">
+        <v/>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>H29568474</v>
+        <v/>
       </c>
       <c r="B7" t="str">
-        <v>terminado</v>
+        <v/>
+      </c>
+      <c r="C7" t="str">
+        <v/>
+      </c>
+      <c r="D7" t="str">
+        <v/>
+      </c>
+      <c r="E7" t="str">
+        <v/>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>H29617552</v>
+        <v/>
       </c>
       <c r="B8" t="str">
-        <v>terminado</v>
+        <v/>
+      </c>
+      <c r="C8" t="str">
+        <v/>
+      </c>
+      <c r="D8" t="str">
+        <v/>
+      </c>
+      <c r="E8" t="str">
+        <v/>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>H29634433</v>
+        <v/>
       </c>
       <c r="B9" t="str">
-        <v>terminado</v>
+        <v/>
+      </c>
+      <c r="C9" t="str">
+        <v/>
+      </c>
+      <c r="D9" t="str">
+        <v/>
+      </c>
+      <c r="E9" t="str">
+        <v/>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>H29674926</v>
+        <v/>
       </c>
       <c r="B10" t="str">
-        <v>terminado</v>
+        <v/>
+      </c>
+      <c r="C10" t="str">
+        <v/>
+      </c>
+      <c r="D10" t="str">
+        <v/>
+      </c>
+      <c r="E10" t="str">
+        <v/>
       </c>
     </row>
     <row r="11">

</xml_diff>

<commit_message>
aañdido verificador de orden logico de visitas para caso 3 ventas 2pdf
</commit_message>
<xml_diff>
--- a/ventas_v2.xlsx
+++ b/ventas_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Fernando\script_ventas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2FE1626-2EC7-499F-A799-8AFDD8439439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5B9220-8FF6-42DC-964A-AEF30FEE5297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,15 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="3">
-  <si>
-    <t>corregir</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="3">
   <si>
     <t/>
   </si>
   <si>
-    <t>H59137216</t>
+    <t>H63420731</t>
+  </si>
+  <si>
+    <t>corregir</t>
   </si>
 </sst>
 </file>
@@ -44,18 +44,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -70,9 +64,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,2699 +408,2773 @@
   <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A11"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.8984375" customWidth="1"/>
-    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="2" max="2" width="25.19921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" t="s">
-        <v>1</v>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
-        <v>1</v>
-      </c>
-      <c r="G5" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" t="s">
-        <v>1</v>
-      </c>
-      <c r="I5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>1</v>
-      </c>
-      <c r="F6" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H6" t="s">
-        <v>1</v>
-      </c>
-      <c r="I6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>1</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>0</v>
+      </c>
       <c r="D11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>1</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>0</v>
+      </c>
       <c r="D13" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>0</v>
+      </c>
       <c r="D14" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
       <c r="C15" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
       <c r="C16" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
       <c r="B17" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H18" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H21" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G22" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H22" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I22" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B24" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G24" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H24" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G25" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H25" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I25" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B26" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C26" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F26" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G26" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H26" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I26" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B27" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C27" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D27" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E27" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F27" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G27" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H27" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I27" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B28" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C28" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F28" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H28" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I28" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B29" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C29" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D29" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E29" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F29" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G29" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H29" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I29" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B30" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C30" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D30" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E30" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F30" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G30" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H30" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I30" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B31" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C31" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D31" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E31" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F31" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G31" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H31" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I31" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B32" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C32" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E32" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F32" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G32" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H32" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I32" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B33" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C33" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D33" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E33" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F33" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G33" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H33" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I33" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B34" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C34" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D34" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E34" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F34" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G34" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H34" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I34" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B35" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C35" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D35" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E35" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F35" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G35" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H35" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I35" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B36" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C36" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D36" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E36" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F36" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G36" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H36" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I36" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B37" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C37" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D37" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E37" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F37" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G37" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H37" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I37" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B38" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C38" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D38" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E38" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F38" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G38" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H38" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I38" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B39" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C39" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D39" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E39" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F39" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G39" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H39" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I39" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B40" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C40" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D40" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E40" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F40" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G40" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H40" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I40" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B41" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C41" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D41" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E41" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F41" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G41" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H41" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I41" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B42" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C42" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D42" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E42" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F42" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G42" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H42" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I42" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B43" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C43" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D43" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E43" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F43" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G43" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H43" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I43" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B44" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C44" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D44" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E44" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F44" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G44" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H44" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I44" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B45" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C45" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D45" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E45" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F45" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G45" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H45" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I45" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B46" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C46" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D46" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E46" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F46" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G46" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H46" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I46" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B47" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C47" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D47" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E47" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F47" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G47" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H47" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I47" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B48" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C48" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D48" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E48" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F48" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G48" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H48" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I48" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B49" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C49" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D49" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E49" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F49" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G49" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H49" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I49" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B50" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C50" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D50" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E50" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F50" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G50" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H50" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I50" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B51" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C51" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D51" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E51" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F51" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G51" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H51" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I51" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B52" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C52" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D52" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E52" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F52" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G52" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H52" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I52" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B53" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C53" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D53" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E53" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F53" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G53" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H53" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I53" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B54" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C54" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D54" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E54" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F54" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G54" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H54" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I54" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B55" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C55" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D55" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E55" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F55" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G55" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H55" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I55" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B56" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C56" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D56" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E56" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F56" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G56" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H56" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I56" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B57" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C57" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D57" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E57" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F57" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G57" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H57" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I57" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B58" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C58" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D58" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E58" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F58" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G58" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H58" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I58" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B59" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C59" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D59" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E59" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F59" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G59" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H59" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I59" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B60" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C60" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D60" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E60" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F60" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G60" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H60" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I60" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B61" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C61" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D61" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E61" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F61" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G61" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H61" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I61" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B62" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C62" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D62" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E62" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F62" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G62" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H62" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I62" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B63" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C63" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D63" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E63" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F63" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G63" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H63" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I63" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B64" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C64" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D64" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E64" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F64" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G64" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H64" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I64" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B65" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C65" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D65" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E65" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F65" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G65" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H65" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I65" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B66" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C66" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D66" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E66" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F66" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G66" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H66" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I66" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B67" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C67" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D67" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E67" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F67" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G67" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H67" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I67" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B68" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C68" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D68" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E68" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F68" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G68" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H68" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I68" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B69" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C69" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D69" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E69" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F69" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G69" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H69" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I69" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B70" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C70" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D70" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E70" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F70" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G70" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H70" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I70" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B71" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C71" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D71" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E71" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F71" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G71" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H71" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I71" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B72" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C72" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D72" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E72" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F72" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G72" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H72" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I72" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B73" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C73" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D73" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E73" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F73" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G73" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H73" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I73" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B74" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C74" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D74" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E74" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F74" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G74" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H74" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I74" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B75" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C75" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D75" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E75" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F75" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G75" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H75" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I75" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B76" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C76" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D76" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E76" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F76" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G76" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H76" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I76" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B77" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C77" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D77" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E77" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F77" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G77" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H77" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I77" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B78" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C78" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D78" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E78" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F78" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G78" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H78" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I78" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B79" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C79" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D79" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E79" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F79" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G79" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H79" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I79" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B80" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C80" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D80" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E80" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F80" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G80" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H80" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I80" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B81" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C81" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D81" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E81" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F81" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G81" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H81" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I81" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B82" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C82" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D82" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E82" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F82" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G82" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H82" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I82" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B83" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C83" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D83" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E83" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F83" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G83" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H83" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I83" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B84" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C84" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D84" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E84" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F84" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G84" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H84" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I84" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B85" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C85" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D85" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E85" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F85" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G85" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H85" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I85" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B86" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C86" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D86" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E86" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F86" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G86" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H86" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I86" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B87" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C87" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D87" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E87" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F87" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G87" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H87" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I87" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B88" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C88" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D88" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E88" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F88" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G88" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H88" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I88" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B89" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C89" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D89" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E89" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F89" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G89" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H89" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I89" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B90" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C90" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D90" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E90" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F90" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G90" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H90" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I90" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B91" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C91" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D91" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E91" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F91" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G91" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H91" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I91" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B92" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C92" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D92" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E92" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F92" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G92" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H92" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I92" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B93" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C93" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D93" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E93" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F93" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G93" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H93" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I93" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B94" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C94" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D94" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E94" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F94" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G94" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H94" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I94" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B95" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C95" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D95" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E95" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F95" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G95" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H95" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I95" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B96" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C96" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D96" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E96" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F96" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G96" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H96" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I96" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B97" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C97" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D97" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E97" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F97" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G97" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H97" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I97" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B98" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C98" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D98" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E98" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F98" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G98" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H98" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I98" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B99" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C99" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D99" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E99" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F99" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G99" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H99" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I99" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B100" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C100" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D100" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E100" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F100" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G100" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H100" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I100" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B101" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C101" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D101" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E101" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F101" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G101" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H101" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I101" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A18:I101 B1:I1 B17:I17 C15:I16 D2:I14" numberStoredAsText="1"/>
+    <ignoredError sqref="A13:I101 D1:I1 C11:I12 D2:I10" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
añdido verificador de orden logico de visitas para caso 3 ventas 2pdf
</commit_message>
<xml_diff>
--- a/ventas_v2.xlsx
+++ b/ventas_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Fernando\script_ventas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5B9220-8FF6-42DC-964A-AEF30FEE5297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C1FAA6-9E29-4357-9425-0C0463885022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,15 +20,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="3">
-  <si>
-    <t/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="7">
   <si>
     <t>H63420731</t>
   </si>
   <si>
     <t>corregir</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>H59334268</t>
+  </si>
+  <si>
+    <t>terminado</t>
+  </si>
+  <si>
+    <t>Caso 3 Ventas 2 Pdf</t>
   </si>
 </sst>
 </file>
@@ -407,2774 +419,2925 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="25.19921875" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
       <c r="D3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
       <c r="D4" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H4" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
       <c r="D8" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G8" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H8" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
       <c r="D9" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G9" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H9" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
       <c r="D10" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G10" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H10" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
       <c r="C11" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G11" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H11" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
       <c r="C12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I12" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F13" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G13" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H13" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I13" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F14" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G14" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H14" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I14" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F15" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G15" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H15" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I15" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F16" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G16" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H16" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I16" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F17" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G17" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H17" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I17" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F18" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G18" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H18" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I18" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I19" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F20" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G20" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H20" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I20" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F21" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G21" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H21" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I21" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F22" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G22" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H22" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I22" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E23" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F23" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G23" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H23" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I23" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E24" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F24" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G24" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H24" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I24" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E25" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F25" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G25" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H25" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I25" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C26" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E26" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F26" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G26" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H26" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I26" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E27" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F27" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G27" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H27" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I27" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D28" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E28" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F28" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G28" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H28" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I28" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B29" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E29" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F29" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G29" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H29" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I29" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D30" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F30" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G30" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H30" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I30" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B31" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E31" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F31" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G31" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H31" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I31" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B32" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D32" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E32" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F32" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G32" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H32" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I32" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D33" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E33" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F33" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G33" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H33" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I33" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C34" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D34" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E34" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F34" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G34" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H34" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I34" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D35" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E35" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F35" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G35" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H35" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I35" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B36" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C36" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D36" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E36" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F36" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G36" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H36" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I36" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B37" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D37" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E37" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F37" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G37" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H37" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I37" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B38" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C38" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D38" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E38" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F38" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G38" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H38" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I38" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B39" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C39" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D39" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E39" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F39" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G39" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H39" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I39" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B40" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C40" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D40" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E40" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F40" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G40" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H40" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I40" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B41" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C41" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D41" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E41" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F41" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G41" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H41" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I41" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B42" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C42" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D42" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E42" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F42" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G42" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H42" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I42" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B43" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C43" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D43" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E43" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F43" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G43" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H43" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I43" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B44" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C44" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D44" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E44" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F44" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G44" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H44" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I44" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B45" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C45" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D45" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E45" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F45" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G45" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H45" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I45" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B46" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C46" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D46" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E46" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F46" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G46" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H46" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I46" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B47" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C47" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D47" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E47" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F47" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G47" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H47" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I47" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B48" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C48" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D48" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E48" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F48" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G48" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H48" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I48" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B49" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C49" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D49" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E49" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F49" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G49" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H49" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I49" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B50" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C50" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D50" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E50" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F50" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G50" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H50" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I50" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B51" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C51" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D51" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E51" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F51" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G51" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H51" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I51" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B52" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C52" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D52" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E52" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F52" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G52" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H52" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I52" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B53" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C53" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D53" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E53" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F53" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G53" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H53" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I53" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B54" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C54" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D54" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E54" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F54" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G54" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H54" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I54" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B55" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C55" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D55" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E55" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F55" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G55" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H55" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I55" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B56" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C56" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D56" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E56" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F56" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G56" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H56" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I56" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B57" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C57" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D57" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E57" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F57" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G57" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H57" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I57" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B58" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C58" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D58" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E58" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F58" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G58" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H58" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I58" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B59" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C59" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D59" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E59" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F59" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G59" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H59" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I59" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B60" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C60" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D60" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E60" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F60" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G60" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H60" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I60" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B61" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C61" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D61" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E61" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F61" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G61" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H61" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I61" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B62" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C62" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D62" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E62" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F62" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G62" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H62" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I62" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B63" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C63" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D63" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E63" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F63" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G63" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H63" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I63" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B64" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C64" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D64" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E64" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F64" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G64" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H64" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I64" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B65" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C65" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D65" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E65" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F65" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G65" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H65" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I65" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B66" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C66" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D66" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E66" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F66" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G66" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H66" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I66" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B67" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C67" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D67" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E67" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F67" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G67" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H67" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I67" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B68" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C68" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D68" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E68" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F68" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G68" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H68" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I68" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B69" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C69" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D69" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E69" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F69" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G69" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H69" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I69" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B70" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C70" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D70" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E70" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F70" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G70" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H70" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I70" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B71" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C71" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D71" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E71" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F71" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G71" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H71" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I71" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B72" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C72" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D72" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E72" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F72" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G72" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H72" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I72" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B73" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C73" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D73" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E73" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F73" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G73" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H73" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I73" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B74" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C74" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D74" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E74" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F74" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G74" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H74" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I74" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B75" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C75" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D75" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E75" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F75" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G75" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H75" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I75" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B76" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C76" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D76" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E76" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F76" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G76" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H76" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I76" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B77" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C77" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D77" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E77" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F77" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G77" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H77" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I77" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B78" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C78" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D78" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E78" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F78" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G78" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H78" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I78" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B79" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C79" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D79" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E79" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F79" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G79" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H79" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I79" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B80" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C80" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D80" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E80" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F80" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G80" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H80" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I80" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B81" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C81" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D81" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E81" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F81" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G81" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H81" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I81" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B82" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C82" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D82" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E82" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F82" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G82" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H82" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I82" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B83" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C83" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D83" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E83" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F83" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G83" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H83" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I83" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B84" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C84" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D84" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E84" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F84" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G84" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H84" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I84" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B85" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C85" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D85" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E85" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F85" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G85" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H85" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I85" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B86" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C86" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D86" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E86" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F86" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G86" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H86" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I86" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B87" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C87" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D87" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E87" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F87" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G87" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H87" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I87" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B88" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C88" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D88" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E88" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F88" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G88" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H88" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I88" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B89" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C89" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D89" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E89" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F89" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G89" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H89" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I89" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B90" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C90" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D90" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E90" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F90" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G90" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H90" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I90" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B91" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C91" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D91" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E91" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F91" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G91" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H91" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I91" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B92" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C92" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D92" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E92" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F92" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G92" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H92" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I92" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B93" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C93" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D93" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E93" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F93" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G93" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H93" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I93" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B94" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C94" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D94" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E94" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F94" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G94" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H94" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I94" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B95" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C95" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D95" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E95" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F95" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G95" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H95" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I95" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B96" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C96" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D96" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E96" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F96" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G96" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H96" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I96" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B97" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C97" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D97" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E97" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F97" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G97" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H97" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I97" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B98" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C98" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D98" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E98" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F98" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G98" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H98" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I98" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B99" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C99" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D99" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E99" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F99" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G99" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H99" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I99" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B100" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C100" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D100" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E100" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F100" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G100" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H100" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I100" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B101" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C101" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D101" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E101" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F101" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G101" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H101" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I101" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A13:I101 D1:I1 C11:I12 D2:I10" numberStoredAsText="1"/>
+    <ignoredError sqref="A2:I101 B1:I1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>